<commit_message>
Finished labeling LLM_corrections_check v2.0
</commit_message>
<xml_diff>
--- a/data/llm_correction_check/llm_correction_checked_2.0.xlsx
+++ b/data/llm_correction_check/llm_correction_checked_2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Dokumente\GitHub Desktop\nonsig-master-thesis\data\llm_correction_check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1066B7-9E21-45A4-B10F-863E4322BC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28D5DDA-4AC3-422E-A93E-37DB82E1C4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2E904296-79A5-4A5C-B72F-CFC29AE77F1A}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="llm_correction_checked" sheetId="1" r:id="rId1"/>
     <sheet name="codebook" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">llm_correction_checked!$A$1:$E$101</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="228">
   <si>
     <t>statement</t>
   </si>
@@ -709,6 +712,27 @@
   </si>
   <si>
     <t>it's basically 'nonsig finding indicates that no change was observed'; strange and incorrect</t>
+  </si>
+  <si>
+    <t>borderline: "not statistically different"; I allow 'statistically' as a synonym for 'significantly' here, knowing that it's not ideal</t>
+  </si>
+  <si>
+    <t>a little strange, but still correct</t>
+  </si>
+  <si>
+    <t>reporting correlations like descriptives, ignoring the significance</t>
+  </si>
+  <si>
+    <t>very tricky; sure, they're compatible with no effect, but also a range of non-zero effects; I count this as a misinterpretation</t>
+  </si>
+  <si>
+    <t>Check code again, little strange</t>
+  </si>
+  <si>
+    <t>Again, it might be consistent with a zero effect, but also with all different kinds of other effects</t>
+  </si>
+  <si>
+    <t>No misinterpretation as no effect, but the LLM removed the p values and reported the effects as descriptives instead? Without the CIs it sounds like the effects were significant…</t>
   </si>
 </sst>
 </file>
@@ -851,7 +875,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1029,6 +1053,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1250,7 +1280,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1277,6 +1307,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1656,9 +1689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC24B177-1069-49AB-B20A-DC9D80522DC8}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2034,7 +2065,7 @@
       <c r="D24" s="8">
         <v>1</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="10" t="s">
         <v>217</v>
       </c>
     </row>
@@ -2297,7 +2328,7 @@
       <c r="D41" s="8">
         <v>1</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="10" t="s">
         <v>220</v>
       </c>
     </row>
@@ -2476,8 +2507,12 @@
       <c r="C53" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D53" s="8"/>
-      <c r="E53" s="4"/>
+      <c r="D53" s="8">
+        <v>0</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
@@ -2489,7 +2524,9 @@
       <c r="C54" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D54" s="8"/>
+      <c r="D54" s="8">
+        <v>0</v>
+      </c>
       <c r="E54" s="4"/>
     </row>
     <row r="55" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -2502,7 +2539,9 @@
       <c r="C55" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D55" s="8"/>
+      <c r="D55" s="8">
+        <v>0</v>
+      </c>
       <c r="E55" s="4"/>
     </row>
     <row r="56" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -2515,7 +2554,9 @@
       <c r="C56" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="D56" s="8"/>
+      <c r="D56" s="8">
+        <v>0</v>
+      </c>
       <c r="E56" s="4"/>
     </row>
     <row r="57" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2528,7 +2569,9 @@
       <c r="C57" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D57" s="8"/>
+      <c r="D57" s="8">
+        <v>0</v>
+      </c>
       <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -2541,7 +2584,9 @@
       <c r="C58" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D58" s="8"/>
+      <c r="D58" s="8">
+        <v>0</v>
+      </c>
       <c r="E58" s="4"/>
     </row>
     <row r="59" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -2554,7 +2599,9 @@
       <c r="C59" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D59" s="8"/>
+      <c r="D59" s="8">
+        <v>0</v>
+      </c>
       <c r="E59" s="4"/>
     </row>
     <row r="60" spans="1:5" ht="135" x14ac:dyDescent="0.25">
@@ -2567,7 +2614,9 @@
       <c r="C60" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D60" s="8"/>
+      <c r="D60" s="8">
+        <v>0</v>
+      </c>
       <c r="E60" s="4"/>
     </row>
     <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2580,7 +2629,9 @@
       <c r="C61" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D61" s="8"/>
+      <c r="D61" s="8">
+        <v>0</v>
+      </c>
       <c r="E61" s="4"/>
     </row>
     <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2593,7 +2644,9 @@
       <c r="C62" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D62" s="8"/>
+      <c r="D62" s="8">
+        <v>0</v>
+      </c>
       <c r="E62" s="4"/>
     </row>
     <row r="63" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2606,8 +2659,12 @@
       <c r="C63" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D63" s="8"/>
-      <c r="E63" s="4"/>
+      <c r="D63" s="8">
+        <v>0</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
@@ -2619,7 +2676,9 @@
       <c r="C64" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D64" s="8"/>
+      <c r="D64" s="8">
+        <v>0</v>
+      </c>
       <c r="E64" s="4"/>
     </row>
     <row r="65" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -2632,7 +2691,9 @@
       <c r="C65" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="D65" s="8"/>
+      <c r="D65" s="8">
+        <v>0</v>
+      </c>
       <c r="E65" s="4"/>
     </row>
     <row r="66" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2645,7 +2706,9 @@
       <c r="C66" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="D66" s="8"/>
+      <c r="D66" s="8">
+        <v>0</v>
+      </c>
       <c r="E66" s="4"/>
     </row>
     <row r="67" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2658,7 +2721,9 @@
       <c r="C67" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D67" s="8"/>
+      <c r="D67" s="8">
+        <v>0</v>
+      </c>
       <c r="E67" s="4"/>
     </row>
     <row r="68" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2671,8 +2736,12 @@
       <c r="C68" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="D68" s="8"/>
-      <c r="E68" s="4"/>
+      <c r="D68" s="8">
+        <v>0</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
@@ -2684,7 +2753,9 @@
       <c r="C69" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="D69" s="8"/>
+      <c r="D69" s="8">
+        <v>0</v>
+      </c>
       <c r="E69" s="4"/>
     </row>
     <row r="70" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2697,7 +2768,9 @@
       <c r="C70" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D70" s="8"/>
+      <c r="D70" s="8">
+        <v>0</v>
+      </c>
       <c r="E70" s="4"/>
     </row>
     <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2710,7 +2783,9 @@
       <c r="C71" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="D71" s="8"/>
+      <c r="D71" s="8">
+        <v>0</v>
+      </c>
       <c r="E71" s="4"/>
     </row>
     <row r="72" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2723,7 +2798,9 @@
       <c r="C72" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D72" s="8"/>
+      <c r="D72" s="8">
+        <v>0</v>
+      </c>
       <c r="E72" s="4"/>
     </row>
     <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2736,7 +2813,9 @@
       <c r="C73" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D73" s="8"/>
+      <c r="D73" s="8">
+        <v>0</v>
+      </c>
       <c r="E73" s="4"/>
     </row>
     <row r="74" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2749,7 +2828,9 @@
       <c r="C74" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="D74" s="8"/>
+      <c r="D74" s="8">
+        <v>0</v>
+      </c>
       <c r="E74" s="4"/>
     </row>
     <row r="75" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -2762,8 +2843,12 @@
       <c r="C75" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="D75" s="8"/>
-      <c r="E75" s="4"/>
+      <c r="D75" s="8">
+        <v>1</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="76" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
@@ -2775,7 +2860,9 @@
       <c r="C76" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D76" s="8"/>
+      <c r="D76" s="8">
+        <v>0</v>
+      </c>
       <c r="E76" s="4"/>
     </row>
     <row r="77" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -2788,7 +2875,9 @@
       <c r="C77" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="D77" s="8"/>
+      <c r="D77" s="8">
+        <v>0</v>
+      </c>
       <c r="E77" s="4"/>
     </row>
     <row r="78" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2801,8 +2890,12 @@
       <c r="C78" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D78" s="8"/>
-      <c r="E78" s="4"/>
+      <c r="D78" s="8">
+        <v>1</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="79" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
@@ -2814,7 +2907,9 @@
       <c r="C79" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D79" s="8"/>
+      <c r="D79" s="8">
+        <v>0</v>
+      </c>
       <c r="E79" s="4"/>
     </row>
     <row r="80" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2827,10 +2922,14 @@
       <c r="C80" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="D80" s="8"/>
-      <c r="E80" s="4"/>
-    </row>
-    <row r="81" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="D80" s="8">
+        <v>1</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>184</v>
       </c>
@@ -2840,8 +2939,12 @@
       <c r="C81" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="D81" s="8"/>
-      <c r="E81" s="4"/>
+      <c r="D81" s="8">
+        <v>1</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="82" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
@@ -2853,7 +2956,9 @@
       <c r="C82" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="D82" s="8"/>
+      <c r="D82" s="8">
+        <v>0</v>
+      </c>
       <c r="E82" s="4"/>
     </row>
     <row r="83" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2866,7 +2971,9 @@
       <c r="C83" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D83" s="8"/>
+      <c r="D83" s="8">
+        <v>0</v>
+      </c>
       <c r="E83" s="4"/>
     </row>
     <row r="84" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2879,7 +2986,9 @@
       <c r="C84" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="D84" s="8"/>
+      <c r="D84" s="8">
+        <v>0</v>
+      </c>
       <c r="E84" s="4"/>
     </row>
     <row r="85" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2892,7 +3001,9 @@
       <c r="C85" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D85" s="8"/>
+      <c r="D85" s="8">
+        <v>0</v>
+      </c>
       <c r="E85" s="4"/>
     </row>
     <row r="86" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2905,7 +3016,9 @@
       <c r="C86" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="D86" s="8"/>
+      <c r="D86" s="8">
+        <v>0</v>
+      </c>
       <c r="E86" s="4"/>
     </row>
     <row r="87" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2918,7 +3031,9 @@
       <c r="C87" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D87" s="8"/>
+      <c r="D87" s="8">
+        <v>0</v>
+      </c>
       <c r="E87" s="4"/>
     </row>
     <row r="88" spans="1:5" ht="150" x14ac:dyDescent="0.25">
@@ -2931,7 +3046,9 @@
       <c r="C88" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D88" s="8"/>
+      <c r="D88" s="8">
+        <v>0</v>
+      </c>
       <c r="E88" s="4"/>
     </row>
     <row r="89" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -2944,7 +3061,9 @@
       <c r="C89" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="D89" s="8"/>
+      <c r="D89" s="8">
+        <v>0</v>
+      </c>
       <c r="E89" s="4"/>
     </row>
     <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2957,7 +3076,9 @@
       <c r="C90" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="D90" s="8"/>
+      <c r="D90" s="8">
+        <v>0</v>
+      </c>
       <c r="E90" s="4"/>
     </row>
     <row r="91" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -2970,7 +3091,9 @@
       <c r="C91" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D91" s="8"/>
+      <c r="D91" s="8">
+        <v>0</v>
+      </c>
       <c r="E91" s="4"/>
     </row>
     <row r="92" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -2983,7 +3106,9 @@
       <c r="C92" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D92" s="8"/>
+      <c r="D92" s="8">
+        <v>0</v>
+      </c>
       <c r="E92" s="4"/>
     </row>
     <row r="93" spans="1:5" ht="105" x14ac:dyDescent="0.25">
@@ -2996,7 +3121,9 @@
       <c r="C93" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="D93" s="8"/>
+      <c r="D93" s="8">
+        <v>0</v>
+      </c>
       <c r="E93" s="4"/>
     </row>
     <row r="94" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -3009,7 +3136,9 @@
       <c r="C94" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D94" s="8"/>
+      <c r="D94" s="8">
+        <v>0</v>
+      </c>
       <c r="E94" s="4"/>
     </row>
     <row r="95" spans="1:5" ht="75" x14ac:dyDescent="0.25">
@@ -3022,7 +3151,9 @@
       <c r="C95" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="D95" s="8"/>
+      <c r="D95" s="8">
+        <v>0</v>
+      </c>
       <c r="E95" s="4"/>
     </row>
     <row r="96" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -3035,7 +3166,9 @@
       <c r="C96" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="D96" s="8"/>
+      <c r="D96" s="8">
+        <v>0</v>
+      </c>
       <c r="E96" s="4"/>
     </row>
     <row r="97" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3048,7 +3181,9 @@
       <c r="C97" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D97" s="8"/>
+      <c r="D97" s="8">
+        <v>0</v>
+      </c>
       <c r="E97" s="4"/>
     </row>
     <row r="98" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -3061,7 +3196,9 @@
       <c r="C98" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="D98" s="8"/>
+      <c r="D98" s="8">
+        <v>0</v>
+      </c>
       <c r="E98" s="4"/>
     </row>
     <row r="99" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -3074,7 +3211,9 @@
       <c r="C99" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="D99" s="8"/>
+      <c r="D99" s="8">
+        <v>0</v>
+      </c>
       <c r="E99" s="4"/>
     </row>
     <row r="100" spans="1:5" ht="90" x14ac:dyDescent="0.25">
@@ -3087,7 +3226,9 @@
       <c r="C100" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="D100" s="8"/>
+      <c r="D100" s="8">
+        <v>0</v>
+      </c>
       <c r="E100" s="4"/>
     </row>
     <row r="101" spans="1:5" ht="135" x14ac:dyDescent="0.25">
@@ -3100,10 +3241,15 @@
       <c r="C101" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="D101" s="8"/>
-      <c r="E101" s="4"/>
+      <c r="D101" s="8">
+        <v>1</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>226</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E101" xr:uid="{DC24B177-1069-49AB-B20A-DC9D80522DC8}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Reviewed labels with Daniel
</commit_message>
<xml_diff>
--- a/data/llm_correction_check/llm_correction_checked_2.0.xlsx
+++ b/data/llm_correction_check/llm_correction_checked_2.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Dokumente\GitHub Desktop\nonsig-master-thesis\data\llm_correction_check\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\Documents\GitHub\nonsig-master-thesis\data\llm_correction_check\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28D5DDA-4AC3-422E-A93E-37DB82E1C4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092ED9D7-38BF-46FE-8B10-3508660D3A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2E904296-79A5-4A5C-B72F-CFC29AE77F1A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2E904296-79A5-4A5C-B72F-CFC29AE77F1A}"/>
   </bookViews>
   <sheets>
     <sheet name="llm_correction_checked" sheetId="1" r:id="rId1"/>
@@ -1057,7 +1057,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="3" tint="0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1280,7 +1280,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1307,6 +1307,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1687,9 +1690,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC24B177-1069-49AB-B20A-DC9D80522DC8}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1716,7 +1722,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1731,7 +1737,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>73</v>
       </c>
@@ -1748,7 +1754,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1763,7 +1769,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1778,7 +1784,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>75</v>
       </c>
@@ -1793,7 +1799,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1808,7 +1814,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1823,7 +1829,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>79</v>
       </c>
@@ -1838,7 +1844,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1853,7 +1859,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>82</v>
       </c>
@@ -1868,7 +1874,7 @@
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1883,7 +1889,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>85</v>
       </c>
@@ -1900,7 +1906,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>87</v>
       </c>
@@ -1915,7 +1921,7 @@
       </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
@@ -1930,7 +1936,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>90</v>
       </c>
@@ -1945,7 +1951,7 @@
       </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1960,7 +1966,7 @@
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>93</v>
       </c>
@@ -1975,7 +1981,7 @@
       </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>95</v>
       </c>
@@ -1990,7 +1996,7 @@
       </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>97</v>
       </c>
@@ -2005,7 +2011,7 @@
       </c>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>11</v>
       </c>
@@ -2022,7 +2028,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>12</v>
       </c>
@@ -2037,7 +2043,7 @@
       </c>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>13</v>
       </c>
@@ -2069,7 +2075,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>14</v>
       </c>
@@ -2084,7 +2090,7 @@
       </c>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>105</v>
       </c>
@@ -2099,7 +2105,7 @@
       </c>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>15</v>
       </c>
@@ -2114,7 +2120,7 @@
       </c>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>16</v>
       </c>
@@ -2129,7 +2135,7 @@
       </c>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
@@ -2144,7 +2150,7 @@
       </c>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>18</v>
       </c>
@@ -2159,7 +2165,7 @@
       </c>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>111</v>
       </c>
@@ -2174,7 +2180,7 @@
       </c>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>113</v>
       </c>
@@ -2191,7 +2197,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>115</v>
       </c>
@@ -2208,7 +2214,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>19</v>
       </c>
@@ -2223,7 +2229,7 @@
       </c>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>20</v>
       </c>
@@ -2238,7 +2244,7 @@
       </c>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>119</v>
       </c>
@@ -2253,7 +2259,7 @@
       </c>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>121</v>
       </c>
@@ -2268,7 +2274,7 @@
       </c>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>21</v>
       </c>
@@ -2283,7 +2289,7 @@
       </c>
       <c r="E38" s="4"/>
     </row>
-    <row r="39" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>22</v>
       </c>
@@ -2300,7 +2306,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>23</v>
       </c>
@@ -2332,7 +2338,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>24</v>
       </c>
@@ -2347,7 +2353,7 @@
       </c>
       <c r="E42" s="4"/>
     </row>
-    <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>129</v>
       </c>
@@ -2362,7 +2368,7 @@
       </c>
       <c r="E43" s="4"/>
     </row>
-    <row r="44" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>25</v>
       </c>
@@ -2377,7 +2383,7 @@
       </c>
       <c r="E44" s="4"/>
     </row>
-    <row r="45" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>26</v>
       </c>
@@ -2392,7 +2398,7 @@
       </c>
       <c r="E45" s="4"/>
     </row>
-    <row r="46" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>27</v>
       </c>
@@ -2407,7 +2413,7 @@
       </c>
       <c r="E46" s="4"/>
     </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>134</v>
       </c>
@@ -2422,7 +2428,7 @@
       </c>
       <c r="E47" s="4"/>
     </row>
-    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>28</v>
       </c>
@@ -2437,7 +2443,7 @@
       </c>
       <c r="E48" s="4"/>
     </row>
-    <row r="49" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>137</v>
       </c>
@@ -2452,7 +2458,7 @@
       </c>
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>29</v>
       </c>
@@ -2467,7 +2473,7 @@
       </c>
       <c r="E50" s="4"/>
     </row>
-    <row r="51" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>140</v>
       </c>
@@ -2482,7 +2488,7 @@
       </c>
       <c r="E51" s="4"/>
     </row>
-    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>142</v>
       </c>
@@ -2497,7 +2503,7 @@
       </c>
       <c r="E52" s="4"/>
     </row>
-    <row r="53" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>144</v>
       </c>
@@ -2514,7 +2520,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>30</v>
       </c>
@@ -2529,7 +2535,7 @@
       </c>
       <c r="E54" s="4"/>
     </row>
-    <row r="55" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>31</v>
       </c>
@@ -2544,7 +2550,7 @@
       </c>
       <c r="E55" s="4"/>
     </row>
-    <row r="56" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>32</v>
       </c>
@@ -2559,7 +2565,7 @@
       </c>
       <c r="E56" s="4"/>
     </row>
-    <row r="57" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>149</v>
       </c>
@@ -2574,7 +2580,7 @@
       </c>
       <c r="E57" s="4"/>
     </row>
-    <row r="58" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>33</v>
       </c>
@@ -2589,7 +2595,7 @@
       </c>
       <c r="E58" s="4"/>
     </row>
-    <row r="59" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>34</v>
       </c>
@@ -2604,7 +2610,7 @@
       </c>
       <c r="E59" s="4"/>
     </row>
-    <row r="60" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>153</v>
       </c>
@@ -2619,7 +2625,7 @@
       </c>
       <c r="E60" s="4"/>
     </row>
-    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>35</v>
       </c>
@@ -2634,7 +2640,7 @@
       </c>
       <c r="E61" s="4"/>
     </row>
-    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>156</v>
       </c>
@@ -2649,7 +2655,7 @@
       </c>
       <c r="E62" s="4"/>
     </row>
-    <row r="63" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>36</v>
       </c>
@@ -2666,7 +2672,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>37</v>
       </c>
@@ -2681,7 +2687,7 @@
       </c>
       <c r="E64" s="4"/>
     </row>
-    <row r="65" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>160</v>
       </c>
@@ -2696,7 +2702,7 @@
       </c>
       <c r="E65" s="4"/>
     </row>
-    <row r="66" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>162</v>
       </c>
@@ -2711,7 +2717,7 @@
       </c>
       <c r="E66" s="4"/>
     </row>
-    <row r="67" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>164</v>
       </c>
@@ -2726,7 +2732,7 @@
       </c>
       <c r="E67" s="4"/>
     </row>
-    <row r="68" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>166</v>
       </c>
@@ -2743,7 +2749,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>38</v>
       </c>
@@ -2758,7 +2764,7 @@
       </c>
       <c r="E69" s="4"/>
     </row>
-    <row r="70" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>169</v>
       </c>
@@ -2773,7 +2779,7 @@
       </c>
       <c r="E70" s="4"/>
     </row>
-    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>39</v>
       </c>
@@ -2788,7 +2794,7 @@
       </c>
       <c r="E71" s="4"/>
     </row>
-    <row r="72" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>40</v>
       </c>
@@ -2803,7 +2809,7 @@
       </c>
       <c r="E72" s="4"/>
     </row>
-    <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>41</v>
       </c>
@@ -2818,7 +2824,7 @@
       </c>
       <c r="E73" s="4"/>
     </row>
-    <row r="74" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>42</v>
       </c>
@@ -2846,11 +2852,11 @@
       <c r="D75" s="8">
         <v>1</v>
       </c>
-      <c r="E75" s="10" t="s">
+      <c r="E75" s="11" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>176</v>
       </c>
@@ -2865,7 +2871,7 @@
       </c>
       <c r="E76" s="4"/>
     </row>
-    <row r="77" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>44</v>
       </c>
@@ -2893,11 +2899,11 @@
       <c r="D78" s="8">
         <v>1</v>
       </c>
-      <c r="E78" s="10" t="s">
+      <c r="E78" s="11" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>180</v>
       </c>
@@ -2925,7 +2931,7 @@
       <c r="D80" s="8">
         <v>1</v>
       </c>
-      <c r="E80" s="10" t="s">
+      <c r="E80" s="11" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2946,7 +2952,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>46</v>
       </c>
@@ -2961,7 +2967,7 @@
       </c>
       <c r="E82" s="4"/>
     </row>
-    <row r="83" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>47</v>
       </c>
@@ -2976,7 +2982,7 @@
       </c>
       <c r="E83" s="4"/>
     </row>
-    <row r="84" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>48</v>
       </c>
@@ -2991,7 +2997,7 @@
       </c>
       <c r="E84" s="4"/>
     </row>
-    <row r="85" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>49</v>
       </c>
@@ -3006,7 +3012,7 @@
       </c>
       <c r="E85" s="4"/>
     </row>
-    <row r="86" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>50</v>
       </c>
@@ -3021,7 +3027,7 @@
       </c>
       <c r="E86" s="4"/>
     </row>
-    <row r="87" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>51</v>
       </c>
@@ -3036,7 +3042,7 @@
       </c>
       <c r="E87" s="4"/>
     </row>
-    <row r="88" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>52</v>
       </c>
@@ -3051,7 +3057,7 @@
       </c>
       <c r="E88" s="4"/>
     </row>
-    <row r="89" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>193</v>
       </c>
@@ -3066,7 +3072,7 @@
       </c>
       <c r="E89" s="4"/>
     </row>
-    <row r="90" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>53</v>
       </c>
@@ -3081,7 +3087,7 @@
       </c>
       <c r="E90" s="4"/>
     </row>
-    <row r="91" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>54</v>
       </c>
@@ -3096,7 +3102,7 @@
       </c>
       <c r="E91" s="4"/>
     </row>
-    <row r="92" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>55</v>
       </c>
@@ -3111,7 +3117,7 @@
       </c>
       <c r="E92" s="4"/>
     </row>
-    <row r="93" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>198</v>
       </c>
@@ -3126,7 +3132,7 @@
       </c>
       <c r="E93" s="4"/>
     </row>
-    <row r="94" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>200</v>
       </c>
@@ -3141,7 +3147,7 @@
       </c>
       <c r="E94" s="4"/>
     </row>
-    <row r="95" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>56</v>
       </c>
@@ -3156,7 +3162,7 @@
       </c>
       <c r="E95" s="4"/>
     </row>
-    <row r="96" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>203</v>
       </c>
@@ -3171,7 +3177,7 @@
       </c>
       <c r="E96" s="4"/>
     </row>
-    <row r="97" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>57</v>
       </c>
@@ -3186,7 +3192,7 @@
       </c>
       <c r="E97" s="4"/>
     </row>
-    <row r="98" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>58</v>
       </c>
@@ -3201,7 +3207,7 @@
       </c>
       <c r="E98" s="4"/>
     </row>
-    <row r="99" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>59</v>
       </c>
@@ -3216,7 +3222,7 @@
       </c>
       <c r="E99" s="4"/>
     </row>
-    <row r="100" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>60</v>
       </c>
@@ -3249,7 +3255,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E101" xr:uid="{DC24B177-1069-49AB-B20A-DC9D80522DC8}"/>
+  <autoFilter ref="A1:E101" xr:uid="{DC24B177-1069-49AB-B20A-DC9D80522DC8}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>